<commit_message>
updated some minor outputs
</commit_message>
<xml_diff>
--- a/Python/output/case-study/FC_SA_FAresults.xlsx
+++ b/Python/output/case-study/FC_SA_FAresults.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/local_ysong3/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/output/case-study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongjis/Documents/GitHub/msp_models_for_adaptive_disaster_relief_logistics_planning/Python/output/case-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899665B-7BE5-9D40-9B91-4085D4B7CE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="17500" tabRatio="500"/>
+    <workbookView xWindow="17800" yWindow="5340" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FC_SA_FAresults" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -94,6 +95,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -361,11 +365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,16 +454,16 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>3130824.2604558999</v>
+        <v>3132666.6752300998</v>
       </c>
       <c r="E4">
-        <v>195525.46190686501</v>
+        <v>195434.692801953</v>
       </c>
       <c r="F4">
-        <v>92.4184441566467</v>
+        <v>94.403269767761202</v>
       </c>
       <c r="G4">
-        <v>4.9943711757659903</v>
+        <v>5.0483090877532897</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -565,16 +569,16 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>3207723.43131663</v>
+        <v>3206690.0685868501</v>
       </c>
       <c r="E9">
-        <v>295751.54152186</v>
+        <v>295806.34573619103</v>
       </c>
       <c r="F9">
-        <v>63.032691001891997</v>
+        <v>60.6284019947052</v>
       </c>
       <c r="G9">
-        <v>5.5594518184661803</v>
+        <v>5.4831590652465803</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>